<commit_message>
Sesiones en otra hoja de excel
</commit_message>
<xml_diff>
--- a/NodeHorarios/Info.xlsx
+++ b/NodeHorarios/Info.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>Nombre</t>
   </si>
@@ -66,6 +67,12 @@
   </si>
   <si>
     <t>Informatica 3</t>
+  </si>
+  <si>
+    <t>Informatica 4</t>
+  </si>
+  <si>
+    <t>Informatica 5</t>
   </si>
 </sst>
 </file>
@@ -459,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +477,7 @@
     <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>5</v>
@@ -490,13 +497,8 @@
       </c>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,17 +529,8 @@
       <c r="L2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -561,15 +554,6 @@
       </c>
       <c r="L3" t="s">
         <v>12</v>
-      </c>
-      <c r="N3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O3">
-        <v>2</v>
-      </c>
-      <c r="P3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -579,4 +563,73 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel refactor, algo falla
</commit_message>
<xml_diff>
--- a/NodeHorarios/Info.xlsx
+++ b/NodeHorarios/Info.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="23">
   <si>
     <t>Nombre</t>
   </si>
@@ -69,10 +69,31 @@
     <t>Informatica 3</t>
   </si>
   <si>
-    <t>Informatica 4</t>
-  </si>
-  <si>
-    <t>Informatica 5</t>
+    <t>Mariano</t>
+  </si>
+  <si>
+    <t>Paloma</t>
+  </si>
+  <si>
+    <t>Jose Manuel</t>
+  </si>
+  <si>
+    <t>Angel</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>ISI</t>
+  </si>
+  <si>
+    <t>PRO</t>
   </si>
 </sst>
 </file>
@@ -466,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,6 +577,74 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>
@@ -567,10 +656,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +704,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -626,7 +715,106 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solapes hecho y excel arreglado
</commit_message>
<xml_diff>
--- a/NodeHorarios/Info.xlsx
+++ b/NodeHorarios/Info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="32">
   <si>
     <t>Nombre</t>
   </si>
@@ -90,6 +90,36 @@
   </si>
   <si>
     <t>Jose Manuel</t>
+  </si>
+  <si>
+    <t>Guillermo</t>
+  </si>
+  <si>
+    <t>Teo</t>
+  </si>
+  <si>
+    <t>Rodrigo</t>
+  </si>
+  <si>
+    <t>MET</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>Gianluca</t>
+  </si>
+  <si>
+    <t>ARQ</t>
+  </si>
+  <si>
+    <t>Informatica 2</t>
   </si>
 </sst>
 </file>
@@ -483,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,6 +643,15 @@
       <c r="H4" t="s">
         <v>18</v>
       </c>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
       <c r="N4" t="s">
         <v>11</v>
       </c>
@@ -702,6 +741,21 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
       <c r="N8" t="s">
         <v>14</v>
       </c>
@@ -713,6 +767,21 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
       <c r="N9" t="s">
         <v>15</v>
       </c>
@@ -724,6 +793,21 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
       <c r="N10" t="s">
         <v>15</v>
       </c>
@@ -735,6 +819,21 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
       <c r="N11" t="s">
         <v>16</v>
       </c>
@@ -746,6 +845,18 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>29</v>
+      </c>
       <c r="N12" t="s">
         <v>16</v>
       </c>
@@ -776,6 +887,127 @@
       </c>
       <c r="P14" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>25</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+      <c r="P15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>25</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>26</v>
+      </c>
+      <c r="O17">
+        <v>2</v>
+      </c>
+      <c r="P17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N18" t="s">
+        <v>26</v>
+      </c>
+      <c r="O18">
+        <v>2</v>
+      </c>
+      <c r="P18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N19" t="s">
+        <v>26</v>
+      </c>
+      <c r="O19">
+        <v>2</v>
+      </c>
+      <c r="P19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
+        <v>27</v>
+      </c>
+      <c r="O20">
+        <v>2</v>
+      </c>
+      <c r="P20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>27</v>
+      </c>
+      <c r="O21">
+        <v>2</v>
+      </c>
+      <c r="P21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
+        <v>27</v>
+      </c>
+      <c r="O22">
+        <v>2</v>
+      </c>
+      <c r="P22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>28</v>
+      </c>
+      <c r="O23">
+        <v>2</v>
+      </c>
+      <c r="P23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>28</v>
+      </c>
+      <c r="O24">
+        <v>2</v>
+      </c>
+      <c r="P24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>30</v>
+      </c>
+      <c r="O25">
+        <v>2</v>
+      </c>
+      <c r="P25" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se puede configurar el numero de horas por dia
</commit_message>
<xml_diff>
--- a/NodeHorarios/Info.xlsx
+++ b/NodeHorarios/Info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="32">
   <si>
     <t>Nombre</t>
   </si>
@@ -513,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26:P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,6 +1010,17 @@
         <v>31</v>
       </c>
     </row>
+    <row r="26" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
+        <v>30</v>
+      </c>
+      <c r="O26">
+        <v>2</v>
+      </c>
+      <c r="P26" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>

</xml_diff>